<commit_message>
Name changed to SF for Singleton File
</commit_message>
<xml_diff>
--- a/dev/backends.xlsx
+++ b/dev/backends.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
   <si>
     <t>exists</t>
   </si>
@@ -81,16 +81,26 @@
   </si>
   <si>
     <t>list_keys</t>
+  </si>
+  <si>
+    <t>clear</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -146,11 +156,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,7 +445,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,6 +569,9 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -573,5 +587,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Auto Complete fix - common OC backend not possible
</commit_message>
<xml_diff>
--- a/dev/backends.xlsx
+++ b/dev/backends.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="24">
   <si>
     <t>exists</t>
   </si>
@@ -84,13 +84,25 @@
   </si>
   <si>
     <t>clear</t>
+  </si>
+  <si>
+    <t>SF</t>
+  </si>
+  <si>
+    <t>list_values</t>
+  </si>
+  <si>
+    <t>relocate</t>
+  </si>
+  <si>
+    <t>about_me</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +113,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -156,12 +176,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,20 +463,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -468,11 +490,14 @@
       <c r="E1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -485,11 +510,14 @@
       <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -502,11 +530,14 @@
       <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="G3" t="s">
+      <c r="F3" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -519,11 +550,14 @@
       <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="G4" t="s">
+      <c r="F4" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -536,54 +570,100 @@
       <c r="E5" t="s">
         <v>18</v>
       </c>
-      <c r="G5" t="s">
+      <c r="F5" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="H5" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F6" s="5"/>
+      <c r="H6" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>9</v>
       </c>
-      <c r="G6" t="s">
+      <c r="F7" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="H7" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>5</v>
       </c>
-      <c r="G7" t="s">
+      <c r="F8" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="H8" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>10</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>10</v>
       </c>
-      <c r="G8" t="s">
+      <c r="F9" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="H9" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H10" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H17" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added operations to OC - list_values and relocate are added
</commit_message>
<xml_diff>
--- a/dev/backends.xlsx
+++ b/dev/backends.xlsx
@@ -102,7 +102,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,8 +125,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -136,6 +162,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -176,13 +208,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,7 +502,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,9 +613,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F6" s="5"/>
-      <c r="H6" s="5" t="s">
+    <row r="6" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="7"/>
+      <c r="H6" s="8" t="s">
         <v>21</v>
       </c>
     </row>
@@ -637,13 +673,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H10" s="5" t="s">
+    <row r="10" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H10" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H11" s="5" t="s">
+    <row r="11" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H11" s="9" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>